<commit_message>
1. Updated TimeLog, 2. Added 3 models: Student, Enrollment, Course with properties
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\HomeWorks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0B2CBD-5CFD-4B6F-9019-903DD560B8D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFA1C82-050E-4EAD-88C7-913B636467B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>HTML/CSS_lesson04</t>
+  </si>
+  <si>
+    <t>RP with EFCore, juhendi järgi</t>
   </si>
 </sst>
 </file>
@@ -1323,13 +1326,14 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.21875" customWidth="1"/>
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.6640625" customWidth="1"/>
     <col min="8" max="8" width="29.88671875" customWidth="1"/>
     <col min="9" max="9" width="3.6640625" customWidth="1"/>
@@ -1713,13 +1717,21 @@
       <c r="A17" s="9">
         <v>11</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="7">
+        <v>43869</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.8125</v>
+      </c>
       <c r="D17" s="8"/>
       <c r="E17" s="6"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>

</xml_diff>

<commit_message>
TimeLog, Created DbInitializer, updated Program.cs and Drop-Database in PM
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\HomeWorks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AA793E-D1E8-4EFF-B21F-99B040BD51CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AA8024-A13D-4118-9F99-B55DDB56B54C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -1325,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54441137-D4FD-4874-9FB8-FB7EE834C62F}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1743,13 +1743,21 @@
       <c r="A18" s="23">
         <v>12</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
+      <c r="B18" s="24">
+        <v>43871</v>
+      </c>
+      <c r="C18" s="25">
+        <v>0.8125</v>
+      </c>
       <c r="D18" s="25"/>
       <c r="E18" s="26"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
+      <c r="G18" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>

</xml_diff>

<commit_message>
changes to Pages/Courses CRUD
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\HomeWorks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211747F9-5763-4AE1-B2AF-5D9694683AE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950DA245-9F99-4BA0-85D9-9A533C197F69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
     <sheet name="Nädal 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Nädal 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -148,6 +149,12 @@
   </si>
   <si>
     <t>RP with EFCore, juhendi järgi</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>üritan commiti tagasi saada</t>
   </si>
 </sst>
 </file>
@@ -1325,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54441137-D4FD-4874-9FB8-FB7EE834C62F}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1796,4 +1803,325 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804C2D8A-CDF6-43FF-96C1-91E48BDA98D5}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="38"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="41"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="49"/>
+      <c r="C4" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="43">
+        <v>43871</v>
+      </c>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="44"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="47"/>
+    </row>
+    <row r="6" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="18">
+        <v>43873</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.9375</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21">
+        <v>70</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>70</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Timelog, added instructors pages, updated all the namespaces
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\HomeWorks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8F8020-7A4D-429A-85D0-D6B47AFCEBCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65579F43-6287-4FE5-AD71-7BD5A8047B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -1819,7 +1819,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1994,9 +1994,11 @@
       <c r="D9" s="8">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6">
+        <v>20</v>
+      </c>
       <c r="F9" s="5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>20</v>
@@ -2011,13 +2013,21 @@
       <c r="A10" s="9">
         <v>4</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="7">
+        <v>43878</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -2143,7 +2153,7 @@
       <c r="E19" s="35"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
Beginning of HW3, adding menus About, Students, Courses, Instructors and Departments. Deleted Privacy
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\HomeWorks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65579F43-6287-4FE5-AD71-7BD5A8047B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F31845-4C56-4DAF-971A-AC3F0C7E2C14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>HW2 lõpuni tegemine</t>
+  </si>
+  <si>
+    <t>HW2 lõpuni tegemine, stopped 7/8</t>
   </si>
 </sst>
 </file>
@@ -1819,7 +1822,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2019,14 +2022,20 @@
       <c r="C10" s="8">
         <v>0.77083333333333337</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
+      <c r="D10" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="E10" s="6">
+        <v>20</v>
+      </c>
+      <c r="F10" s="5">
+        <v>130</v>
+      </c>
       <c r="G10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
@@ -2153,7 +2162,7 @@
       <c r="E19" s="35"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>120</v>
+        <v>250</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
Added DB with data, changed Startup and AppSetting.json
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\HomeWorks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F31845-4C56-4DAF-971A-AC3F0C7E2C14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1659968B-66C6-496A-AD12-27BE3E8FCECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>HW2 lõpuni tegemine, stopped 7/8</t>
+  </si>
+  <si>
+    <t>HW3 start</t>
   </si>
 </sst>
 </file>
@@ -1822,7 +1825,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2044,13 +2047,21 @@
       <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="7">
+        <v>43878</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.88194444444444453</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>

</xml_diff>

<commit_message>
Removed time from enrollment
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\HomeWorks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74533B5-7746-4C85-82BD-1E5C442CED7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56874DF4-2ABC-47FB-8B86-46DEF17E6CE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -2210,7 +2210,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2375,9 +2375,13 @@
       <c r="C9" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8">
+        <v>0.375</v>
+      </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>60</v>
+      </c>
       <c r="G9" s="6" t="s">
         <v>16</v>
       </c>
@@ -2390,12 +2394,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="C10" s="8">
+        <v>0.375</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -2521,7 +2531,7 @@
       <c r="E19" s="35"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
Person Inheritance lisamine, vigade parandused
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\HomeWorks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56874DF4-2ABC-47FB-8B86-46DEF17E6CE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{21179505-766D-4A44-A2BE-F4A0BD4B2581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="Nädal 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="51">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -177,6 +178,18 @@
   </si>
   <si>
     <t>HW3 jätkamine</t>
+  </si>
+  <si>
+    <t>kodutöö üleslaadimine + GP video 1</t>
+  </si>
+  <si>
+    <t>GP video 2</t>
+  </si>
+  <si>
+    <t>GP video 3</t>
+  </si>
+  <si>
+    <t>W5</t>
   </si>
 </sst>
 </file>
@@ -2207,10 +2220,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07ED01CA-374D-44E5-ADBC-2090FD744E32}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2268,7 +2281,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="43">
-        <v>43885</v>
+        <v>43888</v>
       </c>
       <c r="H4" s="43"/>
       <c r="I4" s="43"/>
@@ -2386,8 +2399,12 @@
         <v>16</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="10"/>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
@@ -2397,16 +2414,24 @@
       <c r="C10" s="8">
         <v>0.375</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
+      <c r="D10" s="8">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="E10" s="6">
+        <v>20</v>
+      </c>
+      <c r="F10" s="5">
+        <v>200</v>
+      </c>
       <c r="G10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -2414,40 +2439,86 @@
         <v>5</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="10"/>
+      <c r="C11" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E11" s="6">
+        <v>5</v>
+      </c>
+      <c r="F11" s="5">
+        <v>100</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>6</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="10"/>
+      <c r="B12" s="7">
+        <v>43884</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.65625</v>
+      </c>
+      <c r="E12" s="6">
+        <v>10</v>
+      </c>
+      <c r="F12" s="5">
+        <v>95</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>7</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="C13" s="8">
+        <v>0.6875</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E13" s="6">
+        <v>30</v>
+      </c>
+      <c r="F13" s="5">
+        <v>180</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -2455,13 +2526,25 @@
       <c r="A14" s="9">
         <v>8</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="B14" s="7">
+        <v>43886</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="F14" s="5">
+        <v>90</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
@@ -2469,26 +2552,48 @@
       <c r="A15" s="9">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="B15" s="7">
+        <v>43887</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>20</v>
+      </c>
+      <c r="F15" s="5">
+        <v>160</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>10</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="7">
+        <v>43888</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="D16" s="8"/>
       <c r="E16" s="6"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
@@ -2507,40 +2612,54 @@
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="23">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="9">
         <v>12</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="26"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="27"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="9">
+        <v>13</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="30">
-        <f>SUM(F7:F18)</f>
-        <v>160</v>
-      </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="30">
+        <f>SUM(F7:F19)</f>
+        <v>985</v>
+      </c>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:E20"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>

</xml_diff>